<commit_message>
added extra features and po
</commit_message>
<xml_diff>
--- a/src/test/resources/TestData-PROD.xlsx
+++ b/src/test/resources/TestData-PROD.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="32">
   <si>
     <t>testname</t>
   </si>
@@ -45,6 +45,9 @@
   </si>
   <si>
     <t>To check whether the user can add new employee</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
   <si>
     <t>browser</t>
@@ -1477,7 +1480,7 @@
         <v>8</v>
       </c>
       <c r="E3" t="s" s="2">
-        <v>8</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" ht="13.55" customHeight="1">
@@ -1564,22 +1567,22 @@
         <v>2</v>
       </c>
       <c r="C1" t="s" s="2">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D1" t="s" s="2">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E1" t="s" s="2">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F1" t="s" s="2">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s" s="2">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H1" t="s" s="2">
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" ht="28.8" customHeight="1">
@@ -1587,19 +1590,19 @@
         <v>5</v>
       </c>
       <c r="B2" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C2" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D2" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E2" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F2" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G2" s="2"/>
       <c r="H2" s="13"/>
@@ -1609,35 +1612,35 @@
         <v>5</v>
       </c>
       <c r="B3" t="s" s="2">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="C3" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D3" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E3" t="s" s="2">
+        <v>23</v>
+      </c>
+      <c r="F3" t="s" s="2">
         <v>22</v>
-      </c>
-      <c r="F3" t="s" s="2">
-        <v>21</v>
       </c>
       <c r="G3" s="2"/>
       <c r="H3" s="13"/>
     </row>
     <row r="4" ht="28.8" customHeight="1">
       <c r="A4" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C4" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D4" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E4" s="2"/>
       <c r="F4" s="2"/>
@@ -1646,16 +1649,16 @@
     </row>
     <row r="5" ht="28.8" customHeight="1">
       <c r="A5" t="s" s="2">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s" s="2">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D5" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E5" s="2"/>
       <c r="F5" s="2"/>
@@ -1667,13 +1670,13 @@
         <v>5</v>
       </c>
       <c r="B6" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s" s="2">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="E6" s="2"/>
       <c r="F6" s="2"/>
@@ -1682,16 +1685,16 @@
     </row>
     <row r="7" ht="28.8" customHeight="1">
       <c r="A7" t="s" s="2">
+        <v>30</v>
+      </c>
+      <c r="B7" t="s" s="2">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s" s="2">
+        <v>19</v>
+      </c>
+      <c r="D7" t="s" s="2">
         <v>29</v>
-      </c>
-      <c r="B7" t="s" s="2">
-        <v>24</v>
-      </c>
-      <c r="C7" t="s" s="2">
-        <v>18</v>
-      </c>
-      <c r="D7" t="s" s="2">
-        <v>28</v>
       </c>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -1700,16 +1703,16 @@
     </row>
     <row r="8" ht="28.8" customHeight="1">
       <c r="A8" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D8" t="s" s="2">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -1718,16 +1721,16 @@
     </row>
     <row r="9" ht="34.05" customHeight="1">
       <c r="A9" t="s" s="2">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B9" t="s" s="2">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C9" t="s" s="2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s" s="2">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -1742,16 +1745,16 @@
         <v>7</v>
       </c>
       <c r="C10" t="s" s="2">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D10" t="s" s="2">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E10" t="s" s="2">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F10" t="s" s="2">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G10" s="13"/>
       <c r="H10" s="13"/>

</xml_diff>